<commit_message>
billing date, save contract and fixes added
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mishmurodov\Documents\Digital Service\FSC\Training\devCrmv1\DevCrmRobotv1\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75F00607-3A0B-4109-BCB1-0F2301F726CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3409C1FF-3712-41A5-A09B-825171BEBE5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6045" yWindow="4200" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="23040" windowHeight="12204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
   <si>
     <t>Name</t>
   </si>
@@ -162,13 +162,22 @@
     <t>ProcessABCQueue</t>
   </si>
   <si>
-    <t>UrlCrm</t>
-  </si>
-  <si>
     <t>http://foss219.foss.net:8000/sap(bD1lbiZjPTUwMCZkPW1pbg==)/bc/bsp/sap/crm_ui_start/default.htm</t>
   </si>
   <si>
     <t>CRM PR5 link</t>
+  </si>
+  <si>
+    <t>UrlCrmPR</t>
+  </si>
+  <si>
+    <t>UrlCrmTEC</t>
+  </si>
+  <si>
+    <t>http://foss127.foss.net:8000/sap(bD1lbiZjPTUwMCZkPW1pbg==)/bc/bsp/sap/crm_ui_start/default.htm</t>
+  </si>
+  <si>
+    <t>CRM TEC link</t>
   </si>
 </sst>
 </file>
@@ -556,15 +565,15 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" customWidth="1"/>
+    <col min="1" max="1" width="43.5546875" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="81.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -612,7 +621,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="45">
+    <row r="3" spans="1:26" ht="43.2">
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
@@ -622,7 +631,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="30">
+    <row r="5" spans="1:26" ht="28.8">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -635,16 +644,26 @@
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="C6" t="s">
         <v>46</v>
       </c>
-      <c r="C6" t="s">
-        <v>47</v>
-      </c>
     </row>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1640,9 +1659,10 @@
   <phoneticPr fontId="2"/>
   <hyperlinks>
     <hyperlink ref="B6" r:id="rId1" xr:uid="{912E59D2-E347-4081-BECC-EE3EFBC184E3}"/>
+    <hyperlink ref="B7" r:id="rId2" xr:uid="{B3FFF170-1070-4B72-92EE-7E3FF9CD5C62}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -1654,12 +1674,12 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="75.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1696,7 +1716,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="30">
+    <row r="2" spans="1:26" ht="28.8">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1707,7 +1727,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="45">
+    <row r="3" spans="1:26" ht="43.2">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -1821,7 +1841,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="45">
+    <row r="17" spans="1:3" ht="28.8">
       <c r="A17" t="s">
         <v>40</v>
       </c>
@@ -2817,12 +2837,12 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" customWidth="1"/>
-    <col min="3" max="3" width="60.28515625" customWidth="1"/>
-    <col min="4" max="26" width="65.42578125" customWidth="1"/>
+    <col min="1" max="1" width="31.88671875" customWidth="1"/>
+    <col min="2" max="2" width="30.109375" customWidth="1"/>
+    <col min="3" max="3" width="60.33203125" customWidth="1"/>
+    <col min="4" max="26" width="65.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>